<commit_message>
Wxplicit wait utils and Login page added. Test case for invalid login implemented
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium_Project\OHRM\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4AD0152-C593-494E-8F96-F316C8FD433F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B7550D-67F7-4CA2-A55A-2BE036929FF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>userName</t>
   </si>
@@ -34,6 +34,24 @@
   </si>
   <si>
     <t>Shahdat</t>
+  </si>
+  <si>
+    <t>sajib1234567890</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>dfgdfgfhgfh</t>
+  </si>
+  <si>
+    <t>admin123</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>null</t>
   </si>
 </sst>
 </file>
@@ -77,10 +95,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -362,16 +383,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -383,11 +405,67 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>123456</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>111111</v>
+      </c>
+      <c r="B9" s="2">
+        <v>111111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Empty cell value read from excel sheet added
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium_Project\OHRM\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B7550D-67F7-4CA2-A55A-2BE036929FF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CF1D5B2-131A-4FEC-8C11-12682EFF10E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>userName</t>
   </si>
@@ -51,7 +51,7 @@
     <t>admin</t>
   </si>
   <si>
-    <t>null</t>
+    <t>dkjhdbsdsk</t>
   </si>
 </sst>
 </file>
@@ -385,8 +385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,27 +429,13 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -457,7 +443,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
some validation for invalid login added
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium_Project\OHRM\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CF1D5B2-131A-4FEC-8C11-12682EFF10E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F8AECE-8CA1-4CC0-8517-3472094DF6EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="13">
   <si>
     <t>userName</t>
   </si>
@@ -52,6 +52,18 @@
   </si>
   <si>
     <t>dkjhdbsdsk</t>
+  </si>
+  <si>
+    <t>requiredMsg</t>
+  </si>
+  <si>
+    <t>Required</t>
+  </si>
+  <si>
+    <t>Invalid credentials</t>
+  </si>
+  <si>
+    <t>invalidMsg</t>
   </si>
 </sst>
 </file>
@@ -383,75 +395,133 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D2" sqref="D2:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="2"/>
+    <col min="3" max="3" width="17.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2">
         <v>123456</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>111111</v>
       </c>
       <c r="B9" s="2">
         <v>111111</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Some utilities added + Valid login and basepage added
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium_Project\OHRM\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F8AECE-8CA1-4CC0-8517-3472094DF6EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C68706E4-D807-4E0D-B5D1-C2900D5D0984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="inValidLoginData" sheetId="1" r:id="rId1"/>
+    <sheet name="validLoginData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="13">
   <si>
     <t>userName</t>
   </si>
@@ -397,8 +398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,4 +529,39 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D87AC25-B630-49A7-93B9-4B6B1FD2308F}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Base page essential element verification + sidebar functionality added
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium_Project\OHRM\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C68706E4-D807-4E0D-B5D1-C2900D5D0984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADD3B85-FA2D-4831-B591-10B9E8503946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2985" yWindow="1170" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="inValidLoginData" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Dashboard page elements visibility, elements heading visibility and heading assertion added
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium_Project\OHRM\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADD3B85-FA2D-4831-B591-10B9E8503946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E79214CF-CAD5-45A2-9B16-7AA72C98BCA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2985" yWindow="1170" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="inValidLoginData" sheetId="1" r:id="rId1"/>
     <sheet name="validLoginData" sheetId="2" r:id="rId2"/>
+    <sheet name="dashboardElements" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="27">
   <si>
     <t>userName</t>
   </si>
@@ -65,13 +66,55 @@
   </si>
   <si>
     <t>invalidMsg</t>
+  </si>
+  <si>
+    <t>Element 1 Header</t>
+  </si>
+  <si>
+    <t>Element 2 Header</t>
+  </si>
+  <si>
+    <t>Element 3 Header</t>
+  </si>
+  <si>
+    <t>Element 4 Header</t>
+  </si>
+  <si>
+    <t>Element 5 Header</t>
+  </si>
+  <si>
+    <t>Element 6 Header</t>
+  </si>
+  <si>
+    <t>Element 7 Header</t>
+  </si>
+  <si>
+    <t>Time at Work</t>
+  </si>
+  <si>
+    <t>My Actions</t>
+  </si>
+  <si>
+    <t>Quick Launch</t>
+  </si>
+  <si>
+    <t>Buzz Latest Posts</t>
+  </si>
+  <si>
+    <t>Employees on Leave Today</t>
+  </si>
+  <si>
+    <t>Employee Distribution by Sub Unit</t>
+  </si>
+  <si>
+    <t>Employee Distribution by Location</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,6 +126,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -108,7 +157,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -116,6 +165,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -535,7 +585,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D87AC25-B630-49A7-93B9-4B6B1FD2308F}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -564,4 +614,72 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABDBED03-DCB2-4385-9877-E8A4C7F1E767}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="34.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
full work time calculation added with error
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -1,33 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium_Project\OHRM\src\main\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E79214CF-CAD5-45A2-9B16-7AA72C98BCA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="20490" windowHeight="7695" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="inValidLoginData" sheetId="1" r:id="rId1"/>
     <sheet name="validLoginData" sheetId="2" r:id="rId2"/>
     <sheet name="dashboardElements" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="29">
   <si>
     <t>userName</t>
   </si>
@@ -35,15 +24,27 @@
     <t>password</t>
   </si>
   <si>
+    <t>requiredMsg</t>
+  </si>
+  <si>
+    <t>invalidMsg</t>
+  </si>
+  <si>
     <t>Shahdat</t>
   </si>
   <si>
+    <t>Required</t>
+  </si>
+  <si>
+    <t>Invalid credentials</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
     <t>sajib1234567890</t>
   </si>
   <si>
-    <t>Admin</t>
-  </si>
-  <si>
     <t>dfgdfgfhgfh</t>
   </si>
   <si>
@@ -56,18 +57,6 @@
     <t>dkjhdbsdsk</t>
   </si>
   <si>
-    <t>requiredMsg</t>
-  </si>
-  <si>
-    <t>Required</t>
-  </si>
-  <si>
-    <t>Invalid credentials</t>
-  </si>
-  <si>
-    <t>invalidMsg</t>
-  </si>
-  <si>
     <t>Element 1 Header</t>
   </si>
   <si>
@@ -89,6 +78,9 @@
     <t>Element 7 Header</t>
   </si>
   <si>
+    <t>Punch Time</t>
+  </si>
+  <si>
     <t>Time at Work</t>
   </si>
   <si>
@@ -108,18 +100,33 @@
   </si>
   <si>
     <t>Employee Distribution by Location</t>
+  </si>
+  <si>
+    <t>May 10th at 09:36 PM (GMT 5.5)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+  </numFmts>
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -127,25 +134,356 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -153,31 +491,320 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -226,7 +853,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -261,7 +888,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -435,251 +1062,259 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="A1" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="11.7142857142857" style="4" customWidth="1"/>
+    <col min="2" max="2" width="21.7142857142857" style="4" customWidth="1"/>
+    <col min="3" max="3" width="17.1428571428571" style="4" customWidth="1"/>
+    <col min="4" max="4" width="18.4285714285714" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="9.14285714285714" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" s="2" customFormat="1" spans="1:4">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="4">
+        <v>123456</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4">
+      <c r="C6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="C8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2">
-        <v>123456</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="9" spans="1:4">
+      <c r="A9" s="4">
+        <v>111111</v>
+      </c>
+      <c r="B9" s="4">
+        <v>111111</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="D9" s="4" t="s">
         <v>6</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>111111</v>
-      </c>
-      <c r="B9" s="2">
-        <v>111111</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D87AC25-B630-49A7-93B9-4B6B1FD2308F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="13.2857142857143" customWidth="1"/>
+    <col min="2" max="2" width="13.1428571428571" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABDBED03-DCB2-4385-9877-E8A4C7F1E767}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1428571428571" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="13.1428571428571" customWidth="1"/>
+    <col min="4" max="4" width="18.2857142857143" customWidth="1"/>
+    <col min="5" max="5" width="25.5714285714286" customWidth="1"/>
+    <col min="6" max="7" width="34.8571428571429" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" ht="30" spans="1:8">
+      <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="H1" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="3" t="s">
+    <row r="2" s="1" customFormat="1" spans="1:8">
+      <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="F2" s="1" t="s">
         <v>26</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>